<commit_message>
update for OP sms
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/exporter/accesscnt-daily-bymachine.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/exporter/accesscnt-daily-bymachine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -14,8 +14,11 @@
     <sheet name="_input3" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="c_v" localSheetId="2">OFFSET(_input!$C12,0,0,COUNTA(_input!$A:$A)-2, 1)</definedName>
+    <definedName name="s_v" localSheetId="2">OFFSET(_input!$F12,0,0,COUNTA(_input!$A:$A)-2, 1)</definedName>
+    <definedName name="t_v" localSheetId="2">OFFSET(_input!$D12,0,0,COUNTA(_input!$A:$A)-2, 1)</definedName>
     <definedName name="table1DataSource" localSheetId="2">OFFSET(_input!$C11,0,0,COUNTA(_input!$A:$A)-1, 8)</definedName>
-    <definedName name="trendChartDataSource" localSheetId="2">OFFSET(_input!$C11,0,0,COUNTA(_input!$A:$A)-1, 4)</definedName>
+    <definedName name="y_v" localSheetId="2">OFFSET(_input!$E12,0,0,COUNTA(_input!$A:$A)-2, 1)</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1107,14 +1110,26 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>_input!$C$12</c:f>
+              <c:f>_input!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>今日访问量</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>_input!c_v</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1122,49 +1137,101 @@
                 </c:pt>
               </c:strCache>
             </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>_input!t_v</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>47952</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>_input!$E$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>昨日访问量</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$D$11:$F$11</c:f>
+              <c:f>_input!c_v</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>今日访问量</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>昨日访问量</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>上周同期访问量</c:v>
+                  <c:v>db-crm-pss00.db01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>_input!$D$12:$F$12</c:f>
+              <c:f>_input!y_v</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>47952</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45583</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>136</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="70289280"/>
-        <c:axId val="70290816"/>
-      </c:lineChart>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>_input!$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>上周同期访问量</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>_input!c_v</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>db-crm-pss00.db01</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>_input!s_v</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="85896192"/>
+        <c:axId val="86319872"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="70289280"/>
+        <c:axId val="85896192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,14 +1240,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70290816"/>
+        <c:crossAx val="86319872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70290816"/>
+        <c:axId val="86319872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,7 +1256,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70289280"/>
+        <c:crossAx val="85896192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1207,8 +1274,8 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001232" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001232" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75000000000001266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1589,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
@@ -1758,39 +1825,39 @@
       </c>
       <c r="D28" s="38">
         <f>_input!$I12</f>
-        <v>2369</v>
+        <v>47952</v>
       </c>
       <c r="E28" s="39" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="40">
         <f>_input!$G12</f>
-        <v>5.1971129587784937E-2</v>
+        <v>0</v>
       </c>
       <c r="G28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="41">
         <f>_input!$I12</f>
-        <v>2369</v>
+        <v>47952</v>
       </c>
       <c r="I28" s="42">
         <f>_input!$J12</f>
-        <v>47816</v>
+        <v>47952</v>
       </c>
       <c r="J28" s="39" t="s">
         <v>15</v>
       </c>
       <c r="K28" s="40">
         <f>_input!$H12</f>
-        <v>351.58823529411762</v>
+        <v>0</v>
       </c>
       <c r="L28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="M28" s="43">
         <f>_input!$J12</f>
-        <v>47816</v>
+        <v>47952</v>
       </c>
     </row>
     <row r="37" spans="14:14">
@@ -1837,7 +1904,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2075,28 +2142,26 @@
         <v>47952</v>
       </c>
       <c r="E12" s="19">
-        <f>_input2!$B3</f>
-        <v>45583</v>
+        <v>0</v>
       </c>
       <c r="F12" s="19">
-        <f>_input3!$B3</f>
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <f>IF($E12=0,0,$D12/$E12-1)</f>
-        <v>5.1971129587784937E-2</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" ref="H12:H23" si="0">IF($F12=0,0,$D12/$F12-1)</f>
-        <v>351.58823529411762</v>
+        <v>0</v>
       </c>
       <c r="I12" s="19">
         <f>$D12-$E12</f>
-        <v>2369</v>
+        <v>47952</v>
       </c>
       <c r="J12" s="19">
         <f>$D12-$F12</f>
-        <v>47816</v>
+        <v>47952</v>
       </c>
       <c r="K12">
         <f>SUMIF($D12:$D197,"&gt;0")</f>
@@ -2104,11 +2169,11 @@
       </c>
       <c r="L12">
         <f>SUMIF($E12:$E197,"&gt;0")</f>
-        <v>45583</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <f>SUMIF($F12:$F197,"&gt;0")</f>
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13">

</xml_diff>

<commit_message>
update for BAR chart
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/exporter/accesscnt-daily-bymachine.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/exporter/accesscnt-daily-bymachine.xlsx
@@ -1145,7 +1145,7 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>47952</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1227,11 +1227,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="85896192"/>
-        <c:axId val="86319872"/>
+        <c:axId val="40676736"/>
+        <c:axId val="41165952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85896192"/>
+        <c:axId val="40676736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,14 +1240,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86319872"/>
+        <c:crossAx val="41165952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86319872"/>
+        <c:axId val="41165952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,7 +1256,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85896192"/>
+        <c:crossAx val="40676736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1274,7 +1274,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001277" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001277" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1821,11 +1821,11 @@
       </c>
       <c r="C28" s="23">
         <f>_input!$D12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="D28" s="38">
         <f>_input!$I12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="E28" s="39" t="s">
         <v>15</v>
@@ -1839,11 +1839,11 @@
       </c>
       <c r="H28" s="41">
         <f>_input!$I12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="I28" s="42">
         <f>_input!$J12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="J28" s="39" t="s">
         <v>15</v>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="M28" s="43">
         <f>_input!$J12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="14:14">
@@ -2094,7 +2094,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="3">
-        <v>47952</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2139,12 +2139,14 @@
       </c>
       <c r="D12" s="19">
         <f>$B3</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="E12" s="19">
+        <f>_input2!$B3</f>
         <v>0</v>
       </c>
       <c r="F12" s="19">
+        <f>_input3!$B3</f>
         <v>0</v>
       </c>
       <c r="G12">
@@ -2157,15 +2159,15 @@
       </c>
       <c r="I12" s="19">
         <f>$D12-$E12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="J12" s="19">
         <f>$D12-$F12</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="K12">
         <f>SUMIF($D12:$D197,"&gt;0")</f>
-        <v>47952</v>
+        <v>200</v>
       </c>
       <c r="L12">
         <f>SUMIF($E12:$E197,"&gt;0")</f>
@@ -2567,7 +2569,9 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -2599,7 +2603,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="3">
-        <v>45583</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2617,7 +2621,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2650,7 +2654,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="3">
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>